<commit_message>
Server fixes to work with intended excel templates
</commit_message>
<xml_diff>
--- a/backend/excel_files/users.xlsx
+++ b/backend/excel_files/users.xlsx
@@ -1,129 +1,183 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zoran\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sekretarica\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07730C0C-D97A-48B1-8B51-5E3B6A138F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1371902E-DEA3-4053-943F-7165477222FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{F1002799-821A-4E90-9C1B-7DAB624BAD78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{23F33454-C7B2-4CEE-A269-28E947548EC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
-  <si>
-    <t>Zaposleni</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Sifra admina za ispravku</t>
-  </si>
-  <si>
-    <t>Milica Jurisic</t>
-  </si>
-  <si>
-    <t>Milica Vukomanovic</t>
-  </si>
-  <si>
-    <t>Ivan Grkovic</t>
-  </si>
-  <si>
-    <t>Darko Bzovski</t>
-  </si>
-  <si>
-    <t>Ognjen bozickovic</t>
-  </si>
-  <si>
-    <t>Milica1</t>
-  </si>
-  <si>
-    <t>Milica2</t>
-  </si>
-  <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>Darko</t>
-  </si>
-  <si>
-    <t>Ognjen</t>
-  </si>
-  <si>
-    <t>Milica123</t>
-  </si>
-  <si>
-    <t>Ivan123</t>
-  </si>
-  <si>
-    <t>Darko123</t>
-  </si>
-  <si>
-    <t>Ognjen123</t>
-  </si>
-  <si>
-    <t>Regular</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+  <si>
+    <t>Login name</t>
+  </si>
+  <si>
+    <t>BOJAN</t>
+  </si>
+  <si>
+    <t>Regular user</t>
+  </si>
+  <si>
+    <t>D.PRODANOVIC</t>
+  </si>
+  <si>
+    <t>DBZOVSKI</t>
+  </si>
+  <si>
+    <t>G.MUDRINIC</t>
+  </si>
+  <si>
+    <t>IVAN.G</t>
+  </si>
+  <si>
+    <t>L.TUKELIC</t>
+  </si>
+  <si>
+    <t>M.SAVIC</t>
   </si>
   <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>Nema</t>
-  </si>
-  <si>
-    <t>Ima sifra admin123</t>
-  </si>
-  <si>
-    <t>Aleksa Kacar</t>
-  </si>
-  <si>
-    <t>Aleksa</t>
-  </si>
-  <si>
-    <t>Aleksa123</t>
+    <t>O.MILJEVIC</t>
+  </si>
+  <si>
+    <t>OGNJEN.B</t>
+  </si>
+  <si>
+    <t>S.ALEKSANDROVSKI</t>
+  </si>
+  <si>
+    <t>Sasa</t>
+  </si>
+  <si>
+    <t>User 1</t>
+  </si>
+  <si>
+    <t>User 2</t>
+  </si>
+  <si>
+    <t>User 3</t>
+  </si>
+  <si>
+    <t>Lozinka</t>
+  </si>
+  <si>
+    <t>RWuser1</t>
+  </si>
+  <si>
+    <t>RWuser2</t>
+  </si>
+  <si>
+    <t>RWuser3</t>
+  </si>
+  <si>
+    <t>RWuser4</t>
+  </si>
+  <si>
+    <t>RWuser5</t>
+  </si>
+  <si>
+    <t>RWuser6</t>
+  </si>
+  <si>
+    <t>Admin2</t>
+  </si>
+  <si>
+    <t>Admin1</t>
+  </si>
+  <si>
+    <t>RWuser7</t>
+  </si>
+  <si>
+    <t>RWuser8</t>
+  </si>
+  <si>
+    <t>RWuser9</t>
+  </si>
+  <si>
+    <t>RWuser10</t>
+  </si>
+  <si>
+    <t>RWuser11</t>
+  </si>
+  <si>
+    <t>RWuser12</t>
+  </si>
+  <si>
+    <t>Vrsta korisnika</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF004494"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -153,8 +207,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -184,39 +240,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -268,7 +324,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -379,13 +435,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -394,6 +443,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -458,151 +514,217 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8722AE4C-E4D1-49FD-B166-42BFBD7835B8}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A5E1B1-A5EA-4B5B-8293-6C6EBF011D69}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>